<commit_message>
Updated CAN Bus Data Excel
</commit_message>
<xml_diff>
--- a/CAN Bus Data.xlsx
+++ b/CAN Bus Data.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/Durham/Engineering/Final Year Project/4 Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F539F1-FC1A-554F-8A7F-6A14B84A79D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB329D3-F107-496B-A2D8-7721008065B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data Types" sheetId="3" r:id="rId2"/>
     <sheet name="Info" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CAN Data'!$A$1:$S$42</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="221">
   <si>
     <t>CAN_ID</t>
   </si>
@@ -173,9 +176,6 @@
     <t>Current Limit…</t>
   </si>
   <si>
-    <t>Pack Summe…</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -188,21 +188,6 @@
     <t>cell temps, discharge &amp; chage current limit</t>
   </si>
   <si>
-    <t>CRC Checksum</t>
-  </si>
-  <si>
-    <t>Simulated SOC</t>
-  </si>
-  <si>
-    <t>Custom Flag</t>
-  </si>
-  <si>
-    <t>Pack Resistance</t>
-  </si>
-  <si>
-    <t>unused</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -224,9 +209,6 @@
     <t>cell voltages</t>
   </si>
   <si>
-    <t>MPPT poll</t>
-  </si>
-  <si>
     <t>0x603</t>
   </si>
   <si>
@@ -290,9 +272,6 @@
     <t>Staus Information</t>
   </si>
   <si>
-    <t>Bus (Amps + Volts)</t>
-  </si>
-  <si>
     <t>Velocity (m/s + rpm)</t>
   </si>
   <si>
@@ -423,9 +402,6 @@
   </si>
   <si>
     <t>2*float32</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>uint8_t</t>
@@ -669,9 +645,6 @@
     <t>float32</t>
   </si>
   <si>
-    <t>&lt;not in use any longer?</t>
-  </si>
-  <si>
     <t>telem</t>
   </si>
   <si>
@@ -726,15 +699,6 @@
     <t>CAN_ID (dec)</t>
   </si>
   <si>
-    <t>0x703</t>
-  </si>
-  <si>
-    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
-  </si>
-  <si>
-    <t>for testing</t>
-  </si>
-  <si>
     <t>0x111</t>
   </si>
   <si>
@@ -756,9 +720,6 @@
     <t>power</t>
   </si>
   <si>
-    <t>^ 100+val</t>
-  </si>
-  <si>
     <t>Testbed</t>
   </si>
   <si>
@@ -784,13 +745,97 @@
   </si>
   <si>
     <t>0x1B2</t>
+  </si>
+  <si>
+    <t>0x711</t>
+  </si>
+  <si>
+    <t>0x712</t>
+  </si>
+  <si>
+    <t>Tritium ID</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>Active Motor</t>
+  </si>
+  <si>
+    <t>Error Flags</t>
+  </si>
+  <si>
+    <t>Limit Flags</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Bus Measurement</t>
+  </si>
+  <si>
+    <t>Pack SumV</t>
+  </si>
+  <si>
+    <t>int16 &amp; 2*u_int16 &amp; 2* u_int8</t>
+  </si>
+  <si>
+    <t>BMS Message</t>
+  </si>
+  <si>
+    <t>Maybe MPPT?</t>
+  </si>
+  <si>
+    <t>might be completelly wrong</t>
+  </si>
+  <si>
+    <t>uin</t>
+  </si>
+  <si>
+    <t>iin</t>
+  </si>
+  <si>
+    <t>uout</t>
+  </si>
+  <si>
+    <t>tamb</t>
+  </si>
+  <si>
+    <t>3*u_int16 &amp; u_int8</t>
+  </si>
+  <si>
+    <t>MPPT poll javed</t>
+  </si>
+  <si>
+    <t>MPPT poll woof</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>0x771</t>
+  </si>
+  <si>
+    <t>0x772</t>
+  </si>
+  <si>
+    <t>max bus current</t>
+  </si>
+  <si>
+    <t>Driver Set Speed</t>
+  </si>
+  <si>
+    <t>Driver Set Current</t>
+  </si>
+  <si>
+    <t>flag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -808,13 +853,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFAEAAAA"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -876,15 +914,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -896,17 +931,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="38">
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -926,6 +961,151 @@
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1298,399 +1478,601 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7006E8D-471C-FD46-A1D1-22F26DACF42F}">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26:E28"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="24.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="15" width="10.83203125" style="2"/>
-    <col min="16" max="16" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="9.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.09765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.296875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.8984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>60</v>
+      <c r="P1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="4" t="str">
-        <f t="shared" ref="P2:P25" si="0">IF(ISBLANK(D2),"",1/D2)</f>
-        <v/>
-      </c>
-      <c r="Q2" s="4" t="str">
-        <f t="shared" ref="Q2:Q9" si="1">IF(ISBLANK(D2),"",G2/D2)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <f>HEX2DEC(RIGHT(E2,LEN(E2)-2))</f>
+        <v>246</v>
+      </c>
+      <c r="G2" s="1">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="3">
+        <f>IF(ISBLANK(D2),"",1/D2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>IF(ISBLANK(D2),"",G2/D2)</f>
+        <v>4</v>
+      </c>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q3" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="1">
+        <f>HEX2DEC(RIGHT(E3,LEN(E3)-2))</f>
+        <v>273</v>
+      </c>
+      <c r="G3" s="1">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>185</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.1</v>
+        <v>184</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
       <c r="F4" s="1">
         <f>HEX2DEC(RIGHT(E4,LEN(E4)-2))</f>
+        <v>433</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="1">
+        <f>HEX2DEC(RIGHT(E5,LEN(E5)-2))</f>
+        <v>434</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1">
+        <f>HEX2DEC(RIGHT(E6,LEN(E6)-2))</f>
         <v>1281</v>
       </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4">
-        <f t="shared" si="0"/>
+      <c r="G6" s="1">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="3">
+        <f>IF(ISBLANK(D6),"",1/D6)</f>
         <v>10</v>
       </c>
-      <c r="Q4" s="4">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="Q6" s="3">
+        <f>IF(ISBLANK(D6),"",G6/D6)</f>
+        <v>80</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" ref="F5:F37" si="2">HEX2DEC(RIGHT(E5,LEN(E5)-2))</f>
+      <c r="F7" s="1">
+        <f>HEX2DEC(RIGHT(E7,LEN(E7)-2))</f>
         <v>1282</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="P5" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Q5" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q6" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="2"/>
-        <v>246</v>
       </c>
       <c r="G7" s="1">
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>26</v>
+        <v>217</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="P7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q7" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="P7" s="3">
+        <f>IF(ISBLANK(D7),"",1/D7)</f>
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>IF(ISBLANK(D7),"",G7/D7)</f>
+        <v>16</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q8" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1">
+        <f>HEX2DEC(RIGHT(E8,LEN(E8)-2))</f>
+        <v>1536</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="3">
+        <f>IF(ISBLANK(D8),"",1/D8)</f>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>IF(ISBLANK(D8),"",G8/D8)</f>
+        <v>8</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D9" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="2"/>
-        <v>1536</v>
+        <f>HEX2DEC(RIGHT(E9,LEN(E9)-2))</f>
+        <v>1537</v>
+      </c>
+      <c r="G9" s="1">
+        <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>35</v>
+        <v>198</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>124</v>
+        <v>199</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="P9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="R9" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+      <c r="P9" s="3">
+        <f>IF(ISBLANK(D9),"",1/D9)</f>
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>IF(ISBLANK(D9),"",G9/D9)</f>
+        <v>40</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="2"/>
-        <v>1537</v>
-      </c>
-      <c r="G10" s="2">
-        <v>6</v>
+        <f>HEX2DEC(RIGHT(E10,LEN(E10)-2))</f>
+        <v>1538</v>
+      </c>
+      <c r="G10" s="1">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K10" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="L10" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="M10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P10" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q10" s="4" t="str">
-        <f t="shared" ref="Q10:Q25" si="3">IF(ISBLANK(D10),"",G10/D10)</f>
-        <v/>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="P10" s="3">
+        <f>IF(ISBLANK(D10),"",1/D10)</f>
+        <v>5</v>
+      </c>
+      <c r="Q10" s="3">
+        <f>IF(ISBLANK(D10),"",G10/D10)</f>
+        <v>40</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="2"/>
-        <v>1538</v>
+        <f>HEX2DEC(RIGHT(E11,LEN(E11)-2))</f>
+        <v>1539</v>
       </c>
       <c r="G11" s="1">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>35</v>
@@ -1702,7 +2084,7 @@
         <v>35</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>35</v>
@@ -1713,38 +2095,43 @@
       <c r="O11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q11" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P11" s="3">
+        <f>IF(ISBLANK(D11),"",1/D11)</f>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="3">
+        <f>IF(ISBLANK(D11),"",G11/D11)</f>
+        <v>40</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
-        <v>1539</v>
+        <f>HEX2DEC(RIGHT(E12,LEN(E12)-2))</f>
+        <v>1540</v>
       </c>
       <c r="G12" s="1">
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>35</v>
@@ -1756,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>35</v>
@@ -1767,38 +2154,43 @@
       <c r="O12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q12" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P12" s="3">
+        <f>IF(ISBLANK(D12),"",1/D12)</f>
+        <v>5</v>
+      </c>
+      <c r="Q12" s="3">
+        <f>IF(ISBLANK(D12),"",G12/D12)</f>
+        <v>40</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="2"/>
-        <v>1540</v>
+        <f>HEX2DEC(RIGHT(E13,LEN(E13)-2))</f>
+        <v>1541</v>
       </c>
       <c r="G13" s="1">
         <v>8</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>35</v>
@@ -1810,7 +2202,7 @@
         <v>35</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>35</v>
@@ -1821,37 +2213,43 @@
       <c r="O13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q13" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P13" s="3">
+        <f>IF(ISBLANK(D13),"",1/D13)</f>
+        <v>5</v>
+      </c>
+      <c r="Q13" s="3">
+        <f>IF(ISBLANK(D13),"",G13/D13)</f>
+        <v>40</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D14" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="2"/>
-        <v>1541</v>
+        <f>HEX2DEC(RIGHT(E14,LEN(E14)-2))</f>
+        <v>1542</v>
       </c>
       <c r="G14" s="1">
         <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>35</v>
@@ -1863,7 +2261,7 @@
         <v>35</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>35</v>
@@ -1874,37 +2272,43 @@
       <c r="O14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q14" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P14" s="3">
+        <f>IF(ISBLANK(D14),"",1/D14)</f>
+        <v>5</v>
+      </c>
+      <c r="Q14" s="3">
+        <f>IF(ISBLANK(D14),"",G14/D14)</f>
+        <v>40</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D15" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>1542</v>
+        <f>HEX2DEC(RIGHT(E15,LEN(E15)-2))</f>
+        <v>1543</v>
       </c>
       <c r="G15" s="1">
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>35</v>
@@ -1916,7 +2320,7 @@
         <v>35</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>35</v>
@@ -1927,37 +2331,43 @@
       <c r="O15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q15" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P15" s="3">
+        <f>IF(ISBLANK(D15),"",1/D15)</f>
+        <v>5</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>IF(ISBLANK(D15),"",G15/D15)</f>
+        <v>40</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="2"/>
-        <v>1543</v>
+        <f>HEX2DEC(RIGHT(E16,LEN(E16)-2))</f>
+        <v>1544</v>
       </c>
       <c r="G16" s="1">
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>35</v>
@@ -1969,7 +2379,7 @@
         <v>35</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>35</v>
@@ -1980,37 +2390,43 @@
       <c r="O16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q16" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P16" s="3">
+        <f>IF(ISBLANK(D16),"",1/D16)</f>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3">
+        <f>IF(ISBLANK(D16),"",G16/D16)</f>
+        <v>8</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="2"/>
-        <v>1544</v>
+        <f>HEX2DEC(RIGHT(E17,LEN(E17)-2))</f>
+        <v>1545</v>
       </c>
       <c r="G17" s="1">
         <v>8</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>35</v>
@@ -2022,7 +2438,7 @@
         <v>35</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>35</v>
@@ -2033,37 +2449,43 @@
       <c r="O17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q17" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P17" s="3">
+        <f>IF(ISBLANK(D17),"",1/D17)</f>
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <f>IF(ISBLANK(D17),"",G17/D17)</f>
+        <v>8</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="2"/>
-        <v>1545</v>
+        <f>HEX2DEC(RIGHT(E18,LEN(E18)-2))</f>
+        <v>1546</v>
       </c>
       <c r="G18" s="1">
         <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>35</v>
@@ -2075,7 +2497,7 @@
         <v>35</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>35</v>
@@ -2086,37 +2508,43 @@
       <c r="O18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q18" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P18" s="3">
+        <f>IF(ISBLANK(D18),"",1/D18)</f>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <f>IF(ISBLANK(D18),"",G18/D18)</f>
+        <v>8</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="2"/>
-        <v>1546</v>
+        <f>HEX2DEC(RIGHT(E19,LEN(E19)-2))</f>
+        <v>1547</v>
       </c>
       <c r="G19" s="1">
         <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>35</v>
@@ -2128,7 +2556,7 @@
         <v>35</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>35</v>
@@ -2139,37 +2567,43 @@
       <c r="O19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q19" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P19" s="3">
+        <f>IF(ISBLANK(D19),"",1/D19)</f>
+        <v>1</v>
+      </c>
+      <c r="Q19" s="3">
+        <f>IF(ISBLANK(D19),"",G19/D19)</f>
+        <v>8</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D20" s="1">
+        <v>5</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="2"/>
-        <v>1547</v>
+        <f>HEX2DEC(RIGHT(E20,LEN(E20)-2))</f>
+        <v>1548</v>
       </c>
       <c r="G20" s="1">
         <v>8</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>35</v>
@@ -2181,7 +2615,7 @@
         <v>35</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>35</v>
@@ -2192,37 +2626,43 @@
       <c r="O20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q20" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R20" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P20" s="3">
+        <f>IF(ISBLANK(D20),"",1/D20)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q20" s="3">
+        <f>IF(ISBLANK(D20),"",G20/D20)</f>
+        <v>1.6</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D21" s="1">
+        <v>5</v>
+      </c>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="2"/>
-        <v>1548</v>
+        <f>HEX2DEC(RIGHT(E21,LEN(E21)-2))</f>
+        <v>1549</v>
       </c>
       <c r="G21" s="1">
         <v>8</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>35</v>
@@ -2234,7 +2674,7 @@
         <v>35</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>35</v>
@@ -2245,37 +2685,43 @@
       <c r="O21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P21" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q21" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R21" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P21" s="3">
+        <f>IF(ISBLANK(D21),"",1/D21)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q21" s="3">
+        <f>IF(ISBLANK(D21),"",G21/D21)</f>
+        <v>1.6</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="2"/>
-        <v>1549</v>
+        <f>HEX2DEC(RIGHT(E22,LEN(E22)-2))</f>
+        <v>1550</v>
       </c>
       <c r="G22" s="1">
         <v>8</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>35</v>
@@ -2287,542 +2733,513 @@
         <v>35</v>
       </c>
       <c r="L22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="3">
+        <f>IF(ISBLANK(D22),"",1/D22)</f>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="3">
+        <f>IF(ISBLANK(D22),"",G22/D22)</f>
+        <v>8</v>
+      </c>
+      <c r="R22" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P22" s="4" t="str">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.104</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="1">
+        <f>HEX2DEC(RIGHT(E23,LEN(E23)-2))</f>
+        <v>1792</v>
+      </c>
+      <c r="G23" s="1">
+        <v>6</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P23" s="3">
+        <f>IF(ISBLANK(D23),"",1/D23)</f>
+        <v>9.615384615384615</v>
+      </c>
+      <c r="Q23" s="3">
+        <f>IF(ISBLANK(D23),"",G23/D23)</f>
+        <v>57.692307692307693</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.104</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="1">
+        <f>HEX2DEC(RIGHT(E24,LEN(E24)-2))</f>
+        <v>1793</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P24" s="3">
+        <f>IF(ISBLANK(D24),"",1/D24)</f>
+        <v>9.615384615384615</v>
+      </c>
+      <c r="Q24" s="3">
+        <f>IF(ISBLANK(D24),"",G24/D24)</f>
+        <v>57.692307692307693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.104</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="1">
+        <f>HEX2DEC(RIGHT(E25,LEN(E25)-2))</f>
+        <v>1794</v>
+      </c>
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P25" s="3">
+        <f>IF(ISBLANK(D25),"",1/D25)</f>
+        <v>9.615384615384615</v>
+      </c>
+      <c r="Q25" s="3">
+        <f>IF(ISBLANK(D25),"",G25/D25)</f>
+        <v>76.92307692307692</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="1">
+        <f>HEX2DEC(RIGHT(E26,LEN(E26)-2))</f>
+        <v>1809</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F27" s="1">
+        <f>HEX2DEC(RIGHT(E27,LEN(E27)-2))</f>
+        <v>1810</v>
+      </c>
+      <c r="P27" s="3" t="str">
+        <f>IF(ISBLANK(D27),"",1/D27)</f>
         <v/>
       </c>
-      <c r="Q22" s="4" t="str">
-        <f t="shared" si="3"/>
+      <c r="Q27" s="3" t="str">
+        <f>IF(ISBLANK(D27),"",G27/D27)</f>
         <v/>
       </c>
-      <c r="R22" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="2"/>
-        <v>1550</v>
-      </c>
-      <c r="G23" s="1">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P23" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="R27" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="1">
+        <f>HEX2DEC(RIGHT(E28,LEN(E28)-2))</f>
+        <v>1905</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P28" s="3" t="str">
+        <f>IF(ISBLANK(D28),"",1/D28)</f>
         <v/>
       </c>
-      <c r="Q23" s="4" t="str">
-        <f t="shared" si="3"/>
+      <c r="Q28" s="3" t="str">
+        <f>IF(ISBLANK(D28),"",G28/D28)</f>
         <v/>
       </c>
-      <c r="R23" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q24" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P25" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q25" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0.104</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="2"/>
-        <v>1792</v>
-      </c>
-      <c r="G26" s="1">
-        <v>6</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P26" s="4">
-        <f t="shared" ref="P26" si="4">IF(ISBLANK(D26),"",1/D26)</f>
-        <v>9.615384615384615</v>
-      </c>
-      <c r="Q26" s="4">
-        <f>IF(ISBLANK(D26),"",G26/D26)</f>
-        <v>57.692307692307693</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.104</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="2"/>
-        <v>1793</v>
-      </c>
-      <c r="G27" s="1">
-        <v>6</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P27" s="4">
-        <f>IF(ISBLANK(D27),"",1/D27)</f>
-        <v>9.615384615384615</v>
-      </c>
-      <c r="Q27" s="4">
-        <f>IF(ISBLANK(D27),"",G27/D27)</f>
-        <v>57.692307692307693</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0.104</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="2"/>
-        <v>1794</v>
-      </c>
-      <c r="G28" s="1">
-        <v>8</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P28" s="4">
-        <f>IF(ISBLANK(D28),"",1/D28)</f>
-        <v>9.615384615384615</v>
-      </c>
-      <c r="Q28" s="4">
-        <f>IF(ISBLANK(D28),"",G28/D28)</f>
-        <v>76.92307692307692</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R28" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="1">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P29" s="4" t="str">
+        <v>216</v>
+      </c>
+      <c r="F29" s="1">
+        <f>HEX2DEC(RIGHT(E29,LEN(E29)-2))</f>
+        <v>1906</v>
+      </c>
+      <c r="P29" s="3" t="str">
         <f>IF(ISBLANK(D29),"",1/D29)</f>
         <v/>
       </c>
-      <c r="Q29" s="4" t="str">
+      <c r="Q29" s="3" t="str">
         <f>IF(ISBLANK(D29),"",G29/D29)</f>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="E33" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="2"/>
-        <v>1795</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="2"/>
-        <v>273</v>
-      </c>
-      <c r="G35" s="1">
-        <v>8</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="K36" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F39" s="1">
-        <f>HEX2DEC(RIGHT(E39,LEN(E39)-2))</f>
-        <v>433</v>
-      </c>
-      <c r="G39" s="1">
-        <v>8</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R39" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="R29" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F40" s="1">
-        <f>HEX2DEC(RIGHT(E40,LEN(E40)-2))</f>
-        <v>434</v>
-      </c>
-      <c r="G40" s="1">
-        <v>8</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R40" s="8" t="s">
-        <v>204</v>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="e">
+        <f>HEX2DEC(RIGHT(E31,LEN(E31)-2))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P31" s="3">
+        <f>IF(ISBLANK(D31),"",1/D31)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q31" s="3">
+        <f>IF(ISBLANK(D31),"",G31/D31)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S42" xr:uid="{D7006E8D-471C-FD46-A1D1-22F26DACF42F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S42">
+      <sortCondition ref="E1:E42"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H14 H16:H23 L14:L23 H9 L9:O9 H1:O6 H7:N7 H26:O38 H41:O1048576 H39:H40 L39:L40">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="IN USE">
+  <conditionalFormatting sqref="H13 L8:O8 H32:O1048576 H30:H31 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H26:O29 H1:O3 I6:L6">
+    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A9 A14:A23 A26:A1048576">
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="N">
+  <conditionalFormatting sqref="A2:A8 A13:A22 A26:A1048576">
+    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:K23 I9:I10 J9:K9">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",I9)))</formula>
+  <conditionalFormatting sqref="I8:I9 J8:K8">
+    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:O23">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M11)))</formula>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",K10)))</formula>
+  <conditionalFormatting sqref="M9">
+    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M10)))</formula>
+  <conditionalFormatting sqref="I31:K31">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:K40">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",I40)))</formula>
+  <conditionalFormatting sqref="I30:K30">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:K39">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",I39)))</formula>
+  <conditionalFormatting sqref="M30:O30">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M39:O39">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M39)))</formula>
+  <conditionalFormatting sqref="M31:O31">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M40:O40">
+  <conditionalFormatting sqref="A9:A11">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",A25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",A25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",I23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:O6">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:O7">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("IN USE",M7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2831,801 +3248,801 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>159</v>
       </c>
-      <c r="G11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>169</v>
-      </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>159</v>
-      </c>
-      <c r="G12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>169</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="G18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C22" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D44">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D45">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D48">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D49">
         <v>4</v>
@@ -3634,17 +4051,17 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B31 B33:B49">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3661,107 +4078,107 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+      <c r="C12" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="7" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="9"/>
+      <c r="C17" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="9"/>
+      <c r="C18" s="7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C10" s="8" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="9"/>
+      <c r="C19" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="8" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="9"/>
+      <c r="C20" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="8" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="7" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="C14" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="10"/>
-      <c r="C15" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
-      <c r="C16" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="10"/>
-      <c r="C17" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
-      <c r="C18" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
-      <c r="C19" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
-      <c r="C20" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="8" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CAN Bus Data
</commit_message>
<xml_diff>
--- a/CAN Bus Data.xlsx
+++ b/CAN Bus Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB329D3-F107-496B-A2D8-7721008065B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A754B7-97EF-41C0-9BAB-94CDF9714FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
+    <workbookView xWindow="5760" yWindow="1380" windowWidth="17280" windowHeight="8964" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="222">
   <si>
     <t>CAN_ID</t>
   </si>
@@ -705,21 +705,9 @@
     <t>System status messages</t>
   </si>
   <si>
-    <t>SD fail</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>config</t>
-  </si>
-  <si>
     <t>spare</t>
   </si>
   <si>
-    <t>power</t>
-  </si>
-  <si>
     <t>Testbed</t>
   </si>
   <si>
@@ -828,7 +816,22 @@
     <t>Driver Set Current</t>
   </si>
   <si>
-    <t>flag</t>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Writing to SD</t>
+  </si>
+  <si>
+    <t>GPS Time Obtained</t>
+  </si>
+  <si>
+    <t>Loaded Config</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>ok = 0xFF, not ok = 0x0A</t>
   </si>
 </sst>
 </file>
@@ -941,27 +944,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -1480,9 +1463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7006E8D-471C-FD46-A1D1-22F26DACF42F}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1508,7 +1491,7 @@
     <col min="20" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -1564,7 +1547,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -1581,7 +1564,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="1">
-        <f>HEX2DEC(RIGHT(E2,LEN(E2)-2))</f>
+        <f t="shared" ref="F2:F29" si="0">HEX2DEC(RIGHT(E2,LEN(E2)-2))</f>
         <v>246</v>
       </c>
       <c r="G2" s="1">
@@ -1621,7 +1604,7 @@
       </c>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>178</v>
       </c>
@@ -1632,56 +1615,59 @@
         <v>177</v>
       </c>
       <c r="F3" s="1">
-        <f>HEX2DEC(RIGHT(E3,LEN(E3)-2))</f>
+        <f t="shared" si="0"/>
         <v>273</v>
       </c>
       <c r="G3" s="1">
         <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>220</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F4" s="1">
-        <f>HEX2DEC(RIGHT(E4,LEN(E4)-2))</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="G4" s="1">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>35</v>
@@ -1693,7 +1679,7 @@
         <v>35</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>35</v>
@@ -1708,25 +1694,25 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F5" s="1">
-        <f>HEX2DEC(RIGHT(E5,LEN(E5)-2))</f>
+        <f t="shared" si="0"/>
         <v>434</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>35</v>
@@ -1738,7 +1724,7 @@
         <v>35</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>35</v>
@@ -1750,10 +1736,10 @@
         <v>35</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -1770,14 +1756,14 @@
         <v>57</v>
       </c>
       <c r="F6" s="1">
-        <f>HEX2DEC(RIGHT(E6,LEN(E6)-2))</f>
+        <f t="shared" si="0"/>
         <v>1281</v>
       </c>
       <c r="G6" s="1">
         <v>8</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>35</v>
@@ -1789,7 +1775,7 @@
         <v>35</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>35</v>
@@ -1801,18 +1787,18 @@
         <v>35</v>
       </c>
       <c r="P6" s="3">
-        <f>IF(ISBLANK(D6),"",1/D6)</f>
+        <f t="shared" ref="P6:P25" si="1">IF(ISBLANK(D6),"",1/D6)</f>
         <v>10</v>
       </c>
       <c r="Q6" s="3">
-        <f>IF(ISBLANK(D6),"",G6/D6)</f>
+        <f t="shared" ref="Q6:Q25" si="2">IF(ISBLANK(D6),"",G6/D6)</f>
         <v>80</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -1829,7 +1815,7 @@
         <v>58</v>
       </c>
       <c r="F7" s="1">
-        <f>HEX2DEC(RIGHT(E7,LEN(E7)-2))</f>
+        <f t="shared" si="0"/>
         <v>1282</v>
       </c>
       <c r="G7" s="1">
@@ -1848,7 +1834,7 @@
         <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>35</v>
@@ -1860,18 +1846,18 @@
         <v>35</v>
       </c>
       <c r="P7" s="3">
-        <f>IF(ISBLANK(D7),"",1/D7)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q7" s="3">
-        <f>IF(ISBLANK(D7),"",G7/D7)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -1888,14 +1874,14 @@
         <v>61</v>
       </c>
       <c r="F8" s="1">
-        <f>HEX2DEC(RIGHT(E8,LEN(E8)-2))</f>
+        <f t="shared" si="0"/>
         <v>1536</v>
       </c>
       <c r="G8" s="1">
         <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>35</v>
@@ -1907,7 +1893,7 @@
         <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>35</v>
@@ -1919,18 +1905,18 @@
         <v>35</v>
       </c>
       <c r="P8" s="3">
-        <f>IF(ISBLANK(D8),"",1/D8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q8" s="3">
-        <f>IF(ISBLANK(D8),"",G8/D8)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1947,54 +1933,54 @@
         <v>62</v>
       </c>
       <c r="F9" s="1">
-        <f>HEX2DEC(RIGHT(E9,LEN(E9)-2))</f>
+        <f t="shared" si="0"/>
         <v>1537</v>
       </c>
       <c r="G9" s="1">
         <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P9" s="3">
-        <f>IF(ISBLANK(D9),"",1/D9)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q9" s="3">
-        <f>IF(ISBLANK(D9),"",G9/D9)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
@@ -2006,7 +1992,7 @@
         <v>63</v>
       </c>
       <c r="F10" s="1">
-        <f>HEX2DEC(RIGHT(E10,LEN(E10)-2))</f>
+        <f t="shared" si="0"/>
         <v>1538</v>
       </c>
       <c r="G10" s="1">
@@ -2037,18 +2023,18 @@
         <v>35</v>
       </c>
       <c r="P10" s="3">
-        <f>IF(ISBLANK(D10),"",1/D10)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q10" s="3">
-        <f>IF(ISBLANK(D10),"",G10/D10)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R10" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
@@ -2065,7 +2051,7 @@
         <v>56</v>
       </c>
       <c r="F11" s="1">
-        <f>HEX2DEC(RIGHT(E11,LEN(E11)-2))</f>
+        <f t="shared" si="0"/>
         <v>1539</v>
       </c>
       <c r="G11" s="1">
@@ -2096,18 +2082,18 @@
         <v>35</v>
       </c>
       <c r="P11" s="3">
-        <f>IF(ISBLANK(D11),"",1/D11)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q11" s="3">
-        <f>IF(ISBLANK(D11),"",G11/D11)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2110,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="1">
-        <f>HEX2DEC(RIGHT(E12,LEN(E12)-2))</f>
+        <f t="shared" si="0"/>
         <v>1540</v>
       </c>
       <c r="G12" s="1">
@@ -2155,18 +2141,18 @@
         <v>35</v>
       </c>
       <c r="P12" s="3">
-        <f>IF(ISBLANK(D12),"",1/D12)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q12" s="3">
-        <f>IF(ISBLANK(D12),"",G12/D12)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R12" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -2183,7 +2169,7 @@
         <v>65</v>
       </c>
       <c r="F13" s="1">
-        <f>HEX2DEC(RIGHT(E13,LEN(E13)-2))</f>
+        <f t="shared" si="0"/>
         <v>1541</v>
       </c>
       <c r="G13" s="1">
@@ -2214,18 +2200,18 @@
         <v>35</v>
       </c>
       <c r="P13" s="3">
-        <f>IF(ISBLANK(D13),"",1/D13)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q13" s="3">
-        <f>IF(ISBLANK(D13),"",G13/D13)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2242,7 +2228,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="1">
-        <f>HEX2DEC(RIGHT(E14,LEN(E14)-2))</f>
+        <f t="shared" si="0"/>
         <v>1542</v>
       </c>
       <c r="G14" s="1">
@@ -2273,18 +2259,18 @@
         <v>35</v>
       </c>
       <c r="P14" s="3">
-        <f>IF(ISBLANK(D14),"",1/D14)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q14" s="3">
-        <f>IF(ISBLANK(D14),"",G14/D14)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R14" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -2301,7 +2287,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="1">
-        <f>HEX2DEC(RIGHT(E15,LEN(E15)-2))</f>
+        <f t="shared" si="0"/>
         <v>1543</v>
       </c>
       <c r="G15" s="1">
@@ -2332,18 +2318,18 @@
         <v>35</v>
       </c>
       <c r="P15" s="3">
-        <f>IF(ISBLANK(D15),"",1/D15)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q15" s="3">
-        <f>IF(ISBLANK(D15),"",G15/D15)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2360,7 +2346,7 @@
         <v>68</v>
       </c>
       <c r="F16" s="1">
-        <f>HEX2DEC(RIGHT(E16,LEN(E16)-2))</f>
+        <f t="shared" si="0"/>
         <v>1544</v>
       </c>
       <c r="G16" s="1">
@@ -2391,11 +2377,11 @@
         <v>35</v>
       </c>
       <c r="P16" s="3">
-        <f>IF(ISBLANK(D16),"",1/D16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <f>IF(ISBLANK(D16),"",G16/D16)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R16" s="7" t="s">
@@ -2419,7 +2405,7 @@
         <v>69</v>
       </c>
       <c r="F17" s="1">
-        <f>HEX2DEC(RIGHT(E17,LEN(E17)-2))</f>
+        <f t="shared" si="0"/>
         <v>1545</v>
       </c>
       <c r="G17" s="1">
@@ -2450,11 +2436,11 @@
         <v>35</v>
       </c>
       <c r="P17" s="3">
-        <f>IF(ISBLANK(D17),"",1/D17)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q17" s="3">
-        <f>IF(ISBLANK(D17),"",G17/D17)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R17" s="7" t="s">
@@ -2478,7 +2464,7 @@
         <v>70</v>
       </c>
       <c r="F18" s="1">
-        <f>HEX2DEC(RIGHT(E18,LEN(E18)-2))</f>
+        <f t="shared" si="0"/>
         <v>1546</v>
       </c>
       <c r="G18" s="1">
@@ -2509,11 +2495,11 @@
         <v>35</v>
       </c>
       <c r="P18" s="3">
-        <f>IF(ISBLANK(D18),"",1/D18)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q18" s="3">
-        <f>IF(ISBLANK(D18),"",G18/D18)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R18" s="7" t="s">
@@ -2537,7 +2523,7 @@
         <v>71</v>
       </c>
       <c r="F19" s="1">
-        <f>HEX2DEC(RIGHT(E19,LEN(E19)-2))</f>
+        <f t="shared" si="0"/>
         <v>1547</v>
       </c>
       <c r="G19" s="1">
@@ -2568,11 +2554,11 @@
         <v>35</v>
       </c>
       <c r="P19" s="3">
-        <f>IF(ISBLANK(D19),"",1/D19)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q19" s="3">
-        <f>IF(ISBLANK(D19),"",G19/D19)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R19" s="7" t="s">
@@ -2596,7 +2582,7 @@
         <v>72</v>
       </c>
       <c r="F20" s="1">
-        <f>HEX2DEC(RIGHT(E20,LEN(E20)-2))</f>
+        <f t="shared" si="0"/>
         <v>1548</v>
       </c>
       <c r="G20" s="1">
@@ -2627,11 +2613,11 @@
         <v>35</v>
       </c>
       <c r="P20" s="3">
-        <f>IF(ISBLANK(D20),"",1/D20)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="Q20" s="3">
-        <f>IF(ISBLANK(D20),"",G20/D20)</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="R20" s="7" t="s">
@@ -2655,7 +2641,7 @@
         <v>73</v>
       </c>
       <c r="F21" s="1">
-        <f>HEX2DEC(RIGHT(E21,LEN(E21)-2))</f>
+        <f t="shared" si="0"/>
         <v>1549</v>
       </c>
       <c r="G21" s="1">
@@ -2686,11 +2672,11 @@
         <v>35</v>
       </c>
       <c r="P21" s="3">
-        <f>IF(ISBLANK(D21),"",1/D21)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="Q21" s="3">
-        <f>IF(ISBLANK(D21),"",G21/D21)</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="R21" s="7" t="s">
@@ -2714,7 +2700,7 @@
         <v>74</v>
       </c>
       <c r="F22" s="1">
-        <f>HEX2DEC(RIGHT(E22,LEN(E22)-2))</f>
+        <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="G22" s="1">
@@ -2745,11 +2731,11 @@
         <v>35</v>
       </c>
       <c r="P22" s="3">
-        <f>IF(ISBLANK(D22),"",1/D22)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q22" s="3">
-        <f>IF(ISBLANK(D22),"",G22/D22)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R22" s="7" t="s">
@@ -2773,7 +2759,7 @@
         <v>29</v>
       </c>
       <c r="F23" s="1">
-        <f>HEX2DEC(RIGHT(E23,LEN(E23)-2))</f>
+        <f t="shared" si="0"/>
         <v>1792</v>
       </c>
       <c r="G23" s="1">
@@ -2804,11 +2790,11 @@
         <v>45</v>
       </c>
       <c r="P23" s="3">
-        <f>IF(ISBLANK(D23),"",1/D23)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q23" s="3">
-        <f>IF(ISBLANK(D23),"",G23/D23)</f>
+        <f t="shared" si="2"/>
         <v>57.692307692307693</v>
       </c>
       <c r="R23" s="8" t="s">
@@ -2832,7 +2818,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="1">
-        <f>HEX2DEC(RIGHT(E24,LEN(E24)-2))</f>
+        <f t="shared" si="0"/>
         <v>1793</v>
       </c>
       <c r="G24" s="1">
@@ -2863,11 +2849,11 @@
         <v>45</v>
       </c>
       <c r="P24" s="3">
-        <f>IF(ISBLANK(D24),"",1/D24)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q24" s="3">
-        <f>IF(ISBLANK(D24),"",G24/D24)</f>
+        <f t="shared" si="2"/>
         <v>57.692307692307693</v>
       </c>
     </row>
@@ -2876,7 +2862,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
@@ -2888,7 +2874,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="1">
-        <f>HEX2DEC(RIGHT(E25,LEN(E25)-2))</f>
+        <f t="shared" si="0"/>
         <v>1794</v>
       </c>
       <c r="G25" s="1">
@@ -2907,7 +2893,7 @@
         <v>35</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>35</v>
@@ -2919,15 +2905,15 @@
         <v>46</v>
       </c>
       <c r="P25" s="3">
-        <f>IF(ISBLANK(D25),"",1/D25)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q25" s="3">
-        <f>IF(ISBLANK(D25),"",G25/D25)</f>
+        <f t="shared" si="2"/>
         <v>76.92307692307692</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -2935,22 +2921,22 @@
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F26" s="1">
-        <f>HEX2DEC(RIGHT(E26,LEN(E26)-2))</f>
+        <f t="shared" si="0"/>
         <v>1809</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2958,16 +2944,16 @@
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F27" s="1">
-        <f>HEX2DEC(RIGHT(E27,LEN(E27)-2))</f>
+        <f t="shared" si="0"/>
         <v>1810</v>
       </c>
       <c r="P27" s="3" t="str">
@@ -2979,7 +2965,7 @@
         <v/>
       </c>
       <c r="R27" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2987,38 +2973,38 @@
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F28" s="1">
-        <f>HEX2DEC(RIGHT(E28,LEN(E28)-2))</f>
+        <f t="shared" si="0"/>
         <v>1905</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>45</v>
@@ -3032,10 +3018,10 @@
         <v/>
       </c>
       <c r="R28" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -3043,16 +3029,16 @@
         <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F29" s="1">
-        <f>HEX2DEC(RIGHT(E29,LEN(E29)-2))</f>
+        <f t="shared" si="0"/>
         <v>1906</v>
       </c>
       <c r="P29" s="3" t="str">
@@ -3064,10 +3050,10 @@
         <v/>
       </c>
       <c r="R29" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -3108,133 +3094,133 @@
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H13 L8:O8 H32:O1048576 H30:H31 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H26:O29 H1:O3 I6:L6">
-    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A8 A13:A22 A26:A1048576">
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="32" priority="41" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="30" priority="44" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I9 J8:K8">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="27" priority="36" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:K31">
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="26" priority="35" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:K30">
-    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:O30">
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="24" priority="33" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:O31">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A11">
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:O6">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:O7">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4051,17 +4037,17 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B31 B33:B49">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update GPS Byte data and config file
</commit_message>
<xml_diff>
--- a/CAN Bus Data.xlsx
+++ b/CAN Bus Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB329D3-F107-496B-A2D8-7721008065B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174DABCB-244A-4C50-A81E-6321002FEF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="236">
   <si>
     <t>CAN_ID</t>
   </si>
@@ -90,12 +90,6 @@
   </si>
   <si>
     <t>driver_controls</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>location</t>
   </si>
   <si>
     <t>Tritium</t>
@@ -829,6 +823,57 @@
   </si>
   <si>
     <t>flag</t>
+  </si>
+  <si>
+    <t>TelemetryGPS</t>
+  </si>
+  <si>
+    <t>Date and Time</t>
+  </si>
+  <si>
+    <t>Speed and angle</t>
+  </si>
+  <si>
+    <t>0x0F7</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>0x0F8</t>
+  </si>
+  <si>
+    <t>0x0F9</t>
+  </si>
+  <si>
+    <t>0x0FA</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Alti and Sats</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>float32 &amp; u_uint8</t>
   </si>
 </sst>
 </file>
@@ -941,17 +986,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -1478,11 +1513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7006E8D-471C-FD46-A1D1-22F26DACF42F}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1519,13 +1554,13 @@
         <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
@@ -1555,61 +1590,61 @@
         <v>9</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>219</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
-        <f>HEX2DEC(RIGHT(E2,LEN(E2)-2))</f>
+        <f t="shared" ref="F2:F29" si="0">HEX2DEC(RIGHT(E2,LEN(E2)-2))</f>
         <v>246</v>
       </c>
       <c r="G2" s="1">
         <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P2" s="3">
         <f>IF(ISBLANK(D2),"",1/D2)</f>
@@ -1622,143 +1657,146 @@
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F3" s="1">
-        <f>HEX2DEC(RIGHT(E3,LEN(E3)-2))</f>
+        <f t="shared" si="0"/>
         <v>273</v>
       </c>
       <c r="G3" s="1">
         <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4" s="1">
-        <f>HEX2DEC(RIGHT(E4,LEN(E4)-2))</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="G4" s="1">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F5" s="1">
-        <f>HEX2DEC(RIGHT(E5,LEN(E5)-2))</f>
+        <f t="shared" si="0"/>
         <v>434</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -1767,57 +1805,57 @@
         <v>0.1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1">
-        <f>HEX2DEC(RIGHT(E6,LEN(E6)-2))</f>
+        <f t="shared" si="0"/>
         <v>1281</v>
       </c>
       <c r="G6" s="1">
         <v>8</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P6" s="3">
-        <f>IF(ISBLANK(D6),"",1/D6)</f>
+        <f t="shared" ref="P6:P25" si="1">IF(ISBLANK(D6),"",1/D6)</f>
         <v>10</v>
       </c>
       <c r="Q6" s="3">
-        <f>IF(ISBLANK(D6),"",G6/D6)</f>
+        <f t="shared" ref="Q6:Q25" si="2">IF(ISBLANK(D6),"",G6/D6)</f>
         <v>80</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -1826,942 +1864,942 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1">
-        <f>HEX2DEC(RIGHT(E7,LEN(E7)-2))</f>
+        <f t="shared" si="0"/>
         <v>1282</v>
       </c>
       <c r="G7" s="1">
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P7" s="3">
-        <f>IF(ISBLANK(D7),"",1/D7)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q7" s="3">
-        <f>IF(ISBLANK(D7),"",G7/D7)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1">
-        <f>HEX2DEC(RIGHT(E8,LEN(E8)-2))</f>
+        <f t="shared" si="0"/>
         <v>1536</v>
       </c>
       <c r="G8" s="1">
         <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P8" s="3">
-        <f>IF(ISBLANK(D8),"",1/D8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q8" s="3">
-        <f>IF(ISBLANK(D8),"",G8/D8)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
         <v>0.2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1">
-        <f>HEX2DEC(RIGHT(E9,LEN(E9)-2))</f>
+        <f t="shared" si="0"/>
         <v>1537</v>
       </c>
       <c r="G9" s="1">
         <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P9" s="3">
-        <f>IF(ISBLANK(D9),"",1/D9)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q9" s="3">
-        <f>IF(ISBLANK(D9),"",G9/D9)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>0.2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1">
-        <f>HEX2DEC(RIGHT(E10,LEN(E10)-2))</f>
+        <f t="shared" si="0"/>
         <v>1538</v>
       </c>
       <c r="G10" s="1">
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P10" s="3">
-        <f>IF(ISBLANK(D10),"",1/D10)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q10" s="3">
-        <f>IF(ISBLANK(D10),"",G10/D10)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
         <v>0.2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1">
-        <f>HEX2DEC(RIGHT(E11,LEN(E11)-2))</f>
+        <f t="shared" si="0"/>
         <v>1539</v>
       </c>
       <c r="G11" s="1">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P11" s="3">
-        <f>IF(ISBLANK(D11),"",1/D11)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q11" s="3">
-        <f>IF(ISBLANK(D11),"",G11/D11)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <v>0.2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1">
-        <f>HEX2DEC(RIGHT(E12,LEN(E12)-2))</f>
+        <f t="shared" si="0"/>
         <v>1540</v>
       </c>
       <c r="G12" s="1">
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P12" s="3">
-        <f>IF(ISBLANK(D12),"",1/D12)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q12" s="3">
-        <f>IF(ISBLANK(D12),"",G12/D12)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <v>0.2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1">
-        <f>HEX2DEC(RIGHT(E13,LEN(E13)-2))</f>
+        <f t="shared" si="0"/>
         <v>1541</v>
       </c>
       <c r="G13" s="1">
         <v>8</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P13" s="3">
-        <f>IF(ISBLANK(D13),"",1/D13)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q13" s="3">
-        <f>IF(ISBLANK(D13),"",G13/D13)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1">
         <v>0.2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1">
-        <f>HEX2DEC(RIGHT(E14,LEN(E14)-2))</f>
+        <f t="shared" si="0"/>
         <v>1542</v>
       </c>
       <c r="G14" s="1">
         <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P14" s="3">
-        <f>IF(ISBLANK(D14),"",1/D14)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q14" s="3">
-        <f>IF(ISBLANK(D14),"",G14/D14)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1">
         <v>0.2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F15" s="1">
-        <f>HEX2DEC(RIGHT(E15,LEN(E15)-2))</f>
+        <f t="shared" si="0"/>
         <v>1543</v>
       </c>
       <c r="G15" s="1">
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P15" s="3">
-        <f>IF(ISBLANK(D15),"",1/D15)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q15" s="3">
-        <f>IF(ISBLANK(D15),"",G15/D15)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1">
-        <f>HEX2DEC(RIGHT(E16,LEN(E16)-2))</f>
+        <f t="shared" si="0"/>
         <v>1544</v>
       </c>
       <c r="G16" s="1">
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P16" s="3">
-        <f>IF(ISBLANK(D16),"",1/D16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <f>IF(ISBLANK(D16),"",G16/D16)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R16" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1">
-        <f>HEX2DEC(RIGHT(E17,LEN(E17)-2))</f>
+        <f t="shared" si="0"/>
         <v>1545</v>
       </c>
       <c r="G17" s="1">
         <v>8</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P17" s="3">
-        <f>IF(ISBLANK(D17),"",1/D17)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q17" s="3">
-        <f>IF(ISBLANK(D17),"",G17/D17)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R17" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1">
-        <f>HEX2DEC(RIGHT(E18,LEN(E18)-2))</f>
+        <f t="shared" si="0"/>
         <v>1546</v>
       </c>
       <c r="G18" s="1">
         <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P18" s="3">
-        <f>IF(ISBLANK(D18),"",1/D18)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q18" s="3">
-        <f>IF(ISBLANK(D18),"",G18/D18)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F19" s="1">
-        <f>HEX2DEC(RIGHT(E19,LEN(E19)-2))</f>
+        <f t="shared" si="0"/>
         <v>1547</v>
       </c>
       <c r="G19" s="1">
         <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P19" s="3">
-        <f>IF(ISBLANK(D19),"",1/D19)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q19" s="3">
-        <f>IF(ISBLANK(D19),"",G19/D19)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1">
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1">
-        <f>HEX2DEC(RIGHT(E20,LEN(E20)-2))</f>
+        <f t="shared" si="0"/>
         <v>1548</v>
       </c>
       <c r="G20" s="1">
         <v>8</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P20" s="3">
-        <f>IF(ISBLANK(D20),"",1/D20)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="Q20" s="3">
-        <f>IF(ISBLANK(D20),"",G20/D20)</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="1">
-        <f>HEX2DEC(RIGHT(E21,LEN(E21)-2))</f>
+        <f t="shared" si="0"/>
         <v>1549</v>
       </c>
       <c r="G21" s="1">
         <v>8</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P21" s="3">
-        <f>IF(ISBLANK(D21),"",1/D21)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="Q21" s="3">
-        <f>IF(ISBLANK(D21),"",G21/D21)</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22" s="1">
-        <f>HEX2DEC(RIGHT(E22,LEN(E22)-2))</f>
+        <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="G22" s="1">
         <v>8</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P22" s="3">
-        <f>IF(ISBLANK(D22),"",1/D22)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q22" s="3">
-        <f>IF(ISBLANK(D22),"",G22/D22)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>13</v>
@@ -2770,57 +2808,57 @@
         <v>0.104</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F23" s="1">
-        <f>HEX2DEC(RIGHT(E23,LEN(E23)-2))</f>
+        <f t="shared" si="0"/>
         <v>1792</v>
       </c>
       <c r="G23" s="1">
         <v>6</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P23" s="3">
-        <f>IF(ISBLANK(D23),"",1/D23)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q23" s="3">
-        <f>IF(ISBLANK(D23),"",G23/D23)</f>
+        <f t="shared" si="2"/>
         <v>57.692307692307693</v>
       </c>
       <c r="R23" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>13</v>
@@ -2829,54 +2867,54 @@
         <v>0.104</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1">
-        <f>HEX2DEC(RIGHT(E24,LEN(E24)-2))</f>
+        <f t="shared" si="0"/>
         <v>1793</v>
       </c>
       <c r="G24" s="1">
         <v>6</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="O24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P24" s="3">
-        <f>IF(ISBLANK(D24),"",1/D24)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q24" s="3">
-        <f>IF(ISBLANK(D24),"",G24/D24)</f>
+        <f t="shared" si="2"/>
         <v>57.692307692307693</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
@@ -2885,89 +2923,89 @@
         <v>0.104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F25" s="1">
-        <f>HEX2DEC(RIGHT(E25,LEN(E25)-2))</f>
+        <f t="shared" si="0"/>
         <v>1794</v>
       </c>
       <c r="G25" s="1">
         <v>8</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P25" s="3">
-        <f>IF(ISBLANK(D25),"",1/D25)</f>
+        <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
       <c r="Q25" s="3">
-        <f>IF(ISBLANK(D25),"",G25/D25)</f>
+        <f t="shared" si="2"/>
         <v>76.92307692307692</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F26" s="1">
-        <f>HEX2DEC(RIGHT(E26,LEN(E26)-2))</f>
+        <f t="shared" si="0"/>
         <v>1809</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F27" s="1">
-        <f>HEX2DEC(RIGHT(E27,LEN(E27)-2))</f>
+        <f t="shared" si="0"/>
         <v>1810</v>
       </c>
       <c r="P27" s="3" t="str">
@@ -2979,49 +3017,49 @@
         <v/>
       </c>
       <c r="R27" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F28" s="1">
-        <f>HEX2DEC(RIGHT(E28,LEN(E28)-2))</f>
+        <f t="shared" si="0"/>
         <v>1905</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="2" t="s">
+      <c r="M28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="O28" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P28" s="3" t="str">
         <f>IF(ISBLANK(D28),"",1/D28)</f>
@@ -3032,27 +3070,27 @@
         <v/>
       </c>
       <c r="R28" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F29" s="1">
-        <f>HEX2DEC(RIGHT(E29,LEN(E29)-2))</f>
+        <f t="shared" si="0"/>
         <v>1906</v>
       </c>
       <c r="P29" s="3" t="str">
@@ -3064,10 +3102,10 @@
         <v/>
       </c>
       <c r="R29" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -3076,20 +3114,50 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>18</v>
+        <v>221</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>219</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
-      <c r="F31" s="1" t="e">
+      <c r="E31" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F31" s="1">
         <f>HEX2DEC(RIGHT(E31,LEN(E31)-2))</f>
-        <v>#VALUE!</v>
+        <v>247</v>
+      </c>
+      <c r="G31" s="1">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="P31" s="3">
         <f>IF(ISBLANK(D31),"",1/D31)</f>
@@ -3097,7 +3165,161 @@
       </c>
       <c r="Q31" s="3">
         <f>IF(ISBLANK(D31),"",G31/D31)</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F32" s="1">
+        <f>HEX2DEC(RIGHT(E32,LEN(E32)-2))</f>
+        <v>248</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="P32" s="3">
+        <f t="shared" ref="P32:P35" si="3">IF(ISBLANK(D32),"",1/D32)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" ref="Q32:Q35" si="4">IF(ISBLANK(D32),"",G32/D32)</f>
+        <v>2.5</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" ref="F33:F34" si="5">HEX2DEC(RIGHT(E33,LEN(E33)-2))</f>
+        <v>249</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="G34" s="1">
+        <v>5</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="P34" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P35" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q35" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -3107,135 +3329,135 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H13 L8:O8 H32:O1048576 H30:H31 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H26:O29 H1:O3 I6:L6">
-    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="IN USE">
+  <conditionalFormatting sqref="H13 L8:O8 H35:O1048576 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H26:O29 H1:O3 I6:L6 H30:H34 L32:O34">
+    <cfRule type="containsText" dxfId="35" priority="47" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A8 A13:A22 A26:A1048576">
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="N">
+  <conditionalFormatting sqref="A2:A8 A26:A1048576 A13:A22">
+    <cfRule type="containsText" dxfId="34" priority="43" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="32" priority="46" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I9 J8:K8">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="29" priority="38" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:K31">
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",I31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I30:K30">
-    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="27" priority="36" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:O30">
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="26" priority="35" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M31:O31">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A9:A11">
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",A25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",A25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:O6">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",M6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:O7">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",M7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:K34">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IN USE">
+      <formula>NOT(ISERROR(SEARCH("IN USE",I31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M31:O31">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="IN USE">
-      <formula>NOT(ISERROR(SEARCH("IN USE",M7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("IN USE",M31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3262,367 +3484,367 @@
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" t="s">
         <v>159</v>
       </c>
-      <c r="B10" t="s">
-        <v>161</v>
-      </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -3630,13 +3852,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -3644,13 +3866,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -3658,13 +3880,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
         <v>169</v>
       </c>
-      <c r="B22" t="s">
-        <v>171</v>
-      </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -3672,13 +3894,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -3686,13 +3908,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -3700,13 +3922,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -3714,13 +3936,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -3728,13 +3950,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -3742,13 +3964,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -3756,13 +3978,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -3770,13 +3992,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -3784,13 +4006,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -3798,13 +4020,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -3812,13 +4034,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -3826,13 +4048,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -3840,13 +4062,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D35">
         <v>4</v>
@@ -3854,13 +4076,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -3868,13 +4090,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D37">
         <v>4</v>
@@ -3882,13 +4104,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -3896,13 +4118,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -3910,13 +4132,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -3924,13 +4146,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -3938,13 +4160,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -3952,13 +4174,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -3966,13 +4188,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -3980,13 +4202,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D45">
         <v>4</v>
@@ -3994,13 +4216,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D46">
         <v>4</v>
@@ -4008,13 +4230,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D47">
         <v>4</v>
@@ -4022,13 +4244,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -4036,13 +4258,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D49">
         <v>4</v>
@@ -4051,17 +4273,17 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B31 B33:B49">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IN USE">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4082,103 +4304,103 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C6" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
       <c r="C12" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
       <c r="C13" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
       <c r="C14" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="9"/>
       <c r="C15" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove set pi time using GPS, update MPPT confg
</commit_message>
<xml_diff>
--- a/CAN Bus Data.xlsx
+++ b/CAN Bus Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Telemetry2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A754B7-97EF-41C0-9BAB-94CDF9714FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB41D2-6348-47F5-8070-34DE0E391B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1380" windowWidth="17280" windowHeight="8964" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26B1AE09-9001-5E40-B3F1-E0A864A81904}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="217">
   <si>
     <t>CAN_ID</t>
   </si>
@@ -774,24 +774,6 @@
     <t>Maybe MPPT?</t>
   </si>
   <si>
-    <t>might be completelly wrong</t>
-  </si>
-  <si>
-    <t>uin</t>
-  </si>
-  <si>
-    <t>iin</t>
-  </si>
-  <si>
-    <t>uout</t>
-  </si>
-  <si>
-    <t>tamb</t>
-  </si>
-  <si>
-    <t>3*u_int16 &amp; u_int8</t>
-  </si>
-  <si>
     <t>MPPT poll javed</t>
   </si>
   <si>
@@ -832,6 +814,9 @@
   </si>
   <si>
     <t>ok = 0xFF, not ok = 0x0A</t>
+  </si>
+  <si>
+    <t>4*bit&amp;2*bit&amp;2*bit+u_int8+</t>
   </si>
 </sst>
 </file>
@@ -1463,9 +1448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7006E8D-471C-FD46-A1D1-22F26DACF42F}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1622,19 +1607,19 @@
         <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>179</v>
@@ -1646,7 +1631,7 @@
         <v>179</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1763,7 +1748,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>35</v>
@@ -1775,7 +1760,7 @@
         <v>35</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>35</v>
@@ -1787,7 +1772,7 @@
         <v>35</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" ref="P6:P25" si="1">IF(ISBLANK(D6),"",1/D6)</f>
+        <f t="shared" ref="P6:P26" si="1">IF(ISBLANK(D6),"",1/D6)</f>
         <v>10</v>
       </c>
       <c r="Q6" s="3">
@@ -1834,7 +1819,7 @@
         <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>35</v>
@@ -2388,7 +2373,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -2447,7 +2432,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -2506,7 +2491,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -2565,7 +2550,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -2624,7 +2609,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -2683,7 +2668,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -2742,7 +2727,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
@@ -2801,7 +2786,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
@@ -2857,7 +2842,7 @@
         <v>57.692307692307693</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
@@ -2916,12 +2901,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
@@ -2933,18 +2918,48 @@
         <f t="shared" si="0"/>
         <v>1809</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="G26" s="1">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>51</v>
@@ -2956,6 +2971,33 @@
         <f t="shared" si="0"/>
         <v>1810</v>
       </c>
+      <c r="G27" s="1">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0</v>
+      </c>
       <c r="P27" s="3" t="str">
         <f>IF(ISBLANK(D27),"",1/D27)</f>
         <v/>
@@ -2965,10 +3007,10 @@
         <v/>
       </c>
       <c r="R27" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
@@ -2979,35 +3021,14 @@
         <v>14</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
         <v>1905</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>45</v>
+      <c r="G28" s="1">
+        <v>7</v>
       </c>
       <c r="P28" s="3" t="str">
         <f>IF(ISBLANK(D28),"",1/D28)</f>
@@ -3018,13 +3039,10 @@
         <v/>
       </c>
       <c r="R28" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
@@ -3035,12 +3053,15 @@
         <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
         <v>1906</v>
       </c>
+      <c r="G29" s="1">
+        <v>7</v>
+      </c>
       <c r="P29" s="3" t="str">
         <f>IF(ISBLANK(D29),"",1/D29)</f>
         <v/>
@@ -3049,18 +3070,13 @@
         <f>IF(ISBLANK(D29),"",G29/D29)</f>
         <v/>
       </c>
-      <c r="R29" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -3093,7 +3109,7 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H13 L8:O8 H32:O1048576 H30:H31 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H26:O29 H1:O3 I6:L6">
+  <conditionalFormatting sqref="H13 L8:O8 H32:O1048576 H30:H31 L30:L31 L4:O5 H5:K5 H8 L7 L13:L21 I10:K21 M10:O21 H15:H21 H22:O22 H1:O3 I6:L6 H26:O29">
     <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="IN USE">
       <formula>NOT(ISERROR(SEARCH("IN USE",H1)))</formula>
     </cfRule>

</xml_diff>